<commit_message>
Add import_from_excel function to import rates from Excel file.
</commit_message>
<xml_diff>
--- a/exports/Quote_Davis_Wool_21_06_2025.xlsx
+++ b/exports/Quote_Davis_Wool_21_06_2025.xlsx
@@ -1,41 +1,128 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cjoss\Development\web-dev\term1b\rate-manager-app\exports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD972C-C71F-41F1-B555-864D0F24FCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Quote" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Quote" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+  <si>
+    <t>Customer: Davis Wool</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>POD</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Freight USD</t>
+  </si>
+  <si>
+    <t>OTHC AUD</t>
+  </si>
+  <si>
+    <t>DOC AUD</t>
+  </si>
+  <si>
+    <t>CMR AUD</t>
+  </si>
+  <si>
+    <t>AMS USD</t>
+  </si>
+  <si>
+    <t>LSS USD</t>
+  </si>
+  <si>
+    <t>DTHC</t>
+  </si>
+  <si>
+    <t>Free Time</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>Shekou</t>
+  </si>
+  <si>
+    <t>40HC</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>Collect</t>
+  </si>
+  <si>
+    <t>14 Days</t>
+  </si>
+  <si>
+    <t>Kaohsiung</t>
+  </si>
+  <si>
+    <t>20RE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,82 +141,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,152 +445,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="9" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
-    <col width="9" customWidth="1" min="9" max="9"/>
-    <col width="9" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Customer: Davis Wool</t>
-        </is>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>POL</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>POD</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Container</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Freight USD</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>OTHC AUD</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>DOC AUD</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>CMR AUD</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>AMS USD</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>LSS USD</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>DTHC</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>Free Time</t>
-        </is>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Brisbane</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Shekou</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>40HC</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Collect</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>14 Days</t>
-        </is>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add check for existing rates with replace confirmation.
</commit_message>
<xml_diff>
--- a/exports/Quote_Davis_Wool_21_06_2025.xlsx
+++ b/exports/Quote_Davis_Wool_21_06_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cjoss\Development\web-dev\term1b\rate-manager-app\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD972C-C71F-41F1-B555-864D0F24FCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1798B7B-7157-4519-A8FF-1754E384E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Customer: Davis Wool</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>40HC</t>
-  </si>
-  <si>
-    <t>100</t>
   </si>
   <si>
     <t>200</t>
@@ -449,7 +446,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,29 +510,29 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -543,34 +540,34 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
       <c r="D5">
         <v>500</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>600</v>
+      </c>
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>21</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>